<commit_message>
Fixed missing substrate in 2014 NW SML - see data sheet notes
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Byrnes/2014/NW Shoals Entry 2014/NW Shoals UPC 2014.xlsx
+++ b/raw_data/KEEN ONE/Byrnes/2014/NW Shoals Entry 2014/NW Shoals UPC 2014.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="4660" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2995" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2996" uniqueCount="316">
   <si>
     <t>Didemnum albidum</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2660,11 +2660,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X9747"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="M203" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="M216" sqref="M216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13649,7 +13649,9 @@
       <c r="J208" t="s">
         <v>204</v>
       </c>
-      <c r="O208" s="45"/>
+      <c r="O208" s="45" t="s">
+        <v>25</v>
+      </c>
       <c r="P208" s="3" t="s">
         <v>37</v>
       </c>

</xml_diff>